<commit_message>
removed the hyperparameter dict, instead normal global variables are used
</commit_message>
<xml_diff>
--- a/mnist/results-mnist.xlsx
+++ b/mnist/results-mnist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://radbouduniversiteit-my.sharepoint.com/personal/nemo_ingendaa_ru_nl/Documents/Documenten/School/thesis/softRmax-analysis/mnist/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nemo/Desktop/thesis/softRmax-analysis/mnist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="8_{E77F9308-9DFC-7F48-9712-F4F87B0E4875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8339D5FE-CBF4-1344-B52D-49C3B221EB92}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AF3CD1-BE2F-6B40-A9D9-D624DC8023A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="1380" windowWidth="20260" windowHeight="16880" xr2:uid="{7CDF230F-D82A-4F4E-AAA9-9338F0541A49}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" xr2:uid="{7CDF230F-D82A-4F4E-AAA9-9338F0541A49}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
   <si>
     <t xml:space="preserve">conservative_a: </t>
   </si>
@@ -152,22 +152,43 @@
     <t>BIM attack</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.96850 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.98330 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.97800 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.98510 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.98430 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.9851</t>
+    <t xml:space="preserve">[epoch 1], test_accuracy: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.97580 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[epoch 2], test_accuracy: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.98430 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[epoch 3], test_accuracy: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.97620 </t>
+  </si>
+  <si>
+    <t>[epoch 4], test_accuracy:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.97900 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[epoch 5], test_accuracy: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.98570 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.9857</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> softmax</t>
+  </si>
+  <si>
+    <t>kernel_size</t>
   </si>
 </sst>
 </file>
@@ -255,7 +276,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -267,15 +288,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -295,10 +309,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -601,7 +611,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,7 +625,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2"/>
@@ -627,10 +637,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="4" t="s">
@@ -661,10 +671,10 @@
         <v>10</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="G4" s="7" t="s">
+      <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="2">
         <v>10</v>
       </c>
     </row>
@@ -732,13 +742,13 @@
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="2">
         <v>5</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="2">
         <v>5</v>
       </c>
       <c r="G8" t="s">
@@ -752,7 +762,7 @@
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D9" t="s">
@@ -770,7 +780,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>3</v>
@@ -789,174 +799,185 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="2">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
       <c r="E11" s="2"/>
+      <c r="G11" t="s">
+        <v>50</v>
+      </c>
       <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="E17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="B19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G19" t="s">
         <v>5</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="2"/>
-      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>36</v>
-      </c>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="6"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="4" t="s">
+      <c r="F23" s="5"/>
+      <c r="G23" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="8" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added working fgsm-attack creation and testing
</commit_message>
<xml_diff>
--- a/mnist/results-mnist.xlsx
+++ b/mnist/results-mnist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nemo/Desktop/thesis/softRmax-analysis/mnist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AF3CD1-BE2F-6B40-A9D9-D624DC8023A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5755106B-2D73-F145-B520-91AC1B014234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" xr2:uid="{7CDF230F-D82A-4F4E-AAA9-9338F0541A49}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="24700" windowHeight="19060" xr2:uid="{7CDF230F-D82A-4F4E-AAA9-9338F0541A49}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
   <si>
     <t xml:space="preserve">conservative_a: </t>
   </si>
@@ -71,9 +71,6 @@
     <t>[epoch 5], test_accuracy</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.98130 </t>
-  </si>
-  <si>
     <t>function</t>
   </si>
   <si>
@@ -110,85 +107,73 @@
     <t xml:space="preserve"> 0.05</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.98550 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.98610 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.98840 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.98980 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.9898</t>
-  </si>
-  <si>
-    <t>No attack</t>
-  </si>
-  <si>
     <t xml:space="preserve"> softRmax</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.98100 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.98630 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.98890 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.98880 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.9889</t>
-  </si>
-  <si>
     <t>FGSM attack</t>
   </si>
   <si>
     <t>BIM attack</t>
   </si>
   <si>
-    <t xml:space="preserve">[epoch 1], test_accuracy: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.97580 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[epoch 2], test_accuracy: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.98430 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[epoch 3], test_accuracy: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.97620 </t>
-  </si>
-  <si>
-    <t>[epoch 4], test_accuracy:</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.97900 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[epoch 5], test_accuracy: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.98570 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.9857</t>
-  </si>
-  <si>
     <t xml:space="preserve"> softmax</t>
   </si>
   <si>
     <t>kernel_size</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.97740</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.97870</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.98350</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.97240</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.97610</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.9835</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.992</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.98510</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.98950</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.98920</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.99060</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.99200</t>
+  </si>
+  <si>
+    <t>No attack (3 tries)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.97820</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.98530</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.98890</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.98830</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.9895</t>
   </si>
 </sst>
 </file>
@@ -611,7 +596,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -632,47 +617,47 @@
     </row>
     <row r="2" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2">
         <v>10</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" s="2">
         <v>10</v>
@@ -680,19 +665,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2">
         <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2">
         <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" s="2">
         <v>32</v>
@@ -700,39 +685,39 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2">
         <v>128</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="2">
         <v>128</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H7" s="2">
         <v>128</v>
@@ -740,19 +725,19 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="2">
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="2">
         <v>5</v>
@@ -760,27 +745,27 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>21</v>
-      </c>
       <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>3</v>
@@ -792,126 +777,130 @@
         <v>3</v>
       </c>
       <c r="G10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3</v>
+      </c>
       <c r="G11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="H11" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G13" t="s">
         <v>6</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G14" t="s">
         <v>7</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G15" t="s">
         <v>8</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G16" t="s">
         <v>9</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G17" t="s">
         <v>10</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -924,19 +913,19 @@
         <v>5</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G19" t="s">
         <v>5</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -949,7 +938,7 @@
     </row>
     <row r="22" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="6"/>
@@ -963,22 +952,22 @@
         <v>1</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fgsm and bim attacks are implemented and its comparison figures are created
</commit_message>
<xml_diff>
--- a/mnist/results-mnist.xlsx
+++ b/mnist/results-mnist.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nemo/Desktop/thesis/softRmax-analysis/mnist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5755106B-2D73-F145-B520-91AC1B014234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEA6450B-1888-5C4A-A554-AB980BE933F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="24700" windowHeight="19060" xr2:uid="{7CDF230F-D82A-4F4E-AAA9-9338F0541A49}"/>
+    <workbookView xWindow="3480" yWindow="1820" windowWidth="31580" windowHeight="19060" xr2:uid="{7CDF230F-D82A-4F4E-AAA9-9338F0541A49}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
   <si>
     <t xml:space="preserve">conservative_a: </t>
   </si>
@@ -174,13 +175,49 @@
   </si>
   <si>
     <t xml:space="preserve"> 0.9895</t>
+  </si>
+  <si>
+    <t>Loaded the softRmax network</t>
+  </si>
+  <si>
+    <t>Accuracy of 0 : 99.8%</t>
+  </si>
+  <si>
+    <t>Accuracy of 1 : 99.82%</t>
+  </si>
+  <si>
+    <t>Accuracy of 2 : 99.42%</t>
+  </si>
+  <si>
+    <t>Accuracy of 3 : 99.8%</t>
+  </si>
+  <si>
+    <t>Accuracy of 4 : 99.29%</t>
+  </si>
+  <si>
+    <t>Accuracy of 5 : 99.1%</t>
+  </si>
+  <si>
+    <t>Accuracy of 6 : 98.85%</t>
+  </si>
+  <si>
+    <t>Accuracy of 7 : 98.93%</t>
+  </si>
+  <si>
+    <t>Accuracy of 8 : 99.28%</t>
+  </si>
+  <si>
+    <t>Accuracy of 9 : 98.71%</t>
+  </si>
+  <si>
+    <t>Total Accuracy: 99.31%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -227,6 +264,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -261,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -278,6 +327,8 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40A11AE0-B146-4F40-BD5E-14A3A0645060}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,20 +658,21 @@
     <col min="5" max="5" width="12.83203125" customWidth="1"/>
     <col min="7" max="7" width="25.33203125" customWidth="1"/>
     <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="10" max="10" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -641,8 +693,11 @@
       <c r="H3" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J3" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -662,8 +717,11 @@
       <c r="H4" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J4" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -682,8 +740,11 @@
       <c r="H5" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J5" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -702,8 +763,11 @@
       <c r="H6" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J6" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -722,8 +786,11 @@
       <c r="H7" s="2">
         <v>128</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J7" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -742,8 +809,11 @@
       <c r="H8" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J8" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -762,8 +832,11 @@
       <c r="H9" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J9" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -782,8 +855,11 @@
       <c r="H10" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J10" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -802,8 +878,16 @@
       <c r="H11" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J11" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="J12" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -822,8 +906,11 @@
       <c r="H13" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J13" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -842,8 +929,11 @@
       <c r="H14" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J14" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -862,8 +952,9 @@
       <c r="H15" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J15" s="11"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -882,8 +973,9 @@
       <c r="H16" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -902,13 +994,14 @@
       <c r="H17" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J17" s="11"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
       <c r="E18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -928,15 +1021,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -944,7 +1037,7 @@
       <c r="C22" s="6"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>2</v>
       </c>

</xml_diff>